<commit_message>
create 8 wc lang models for the SBML test suite; and update one used to test validation
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/validation/cases/semantic/00001/00001-wc_lang.xlsx
+++ b/tests/multialgorithm/fixtures/validation/cases/semantic/00001/00001-wc_lang.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/multialgorithm/fixtures/validation/cases/semantic/00001/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/multialgorithm/fixtures/validation/testing/semantic/00001/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-26720" yWindow="1920" windowWidth="23700" windowHeight="11840" tabRatio="989" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="1700" windowWidth="23700" windowHeight="11840" tabRatio="989" firstSheet="6" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
   <si>
     <t>Id</t>
   </si>
@@ -314,9 +314,6 @@
     <t>reaction 1</t>
   </si>
   <si>
-    <t>k1 * S1[c] * compartment</t>
-  </si>
-  <si>
     <t>k1</t>
   </si>
   <si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t>Equal MWs mass-balance the reactions</t>
+  </si>
+  <si>
+    <t>k1 * S1[c]</t>
   </si>
 </sst>
 </file>
@@ -882,7 +882,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -927,7 +927,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1031,7 +1031,7 @@
   <sheetPr codeName="Sheet13" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1043,7 +1043,7 @@
     <col min="4" max="4" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1083,6 +1083,9 @@
       <c r="C2" t="s">
         <v>71</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="E2" s="2">
         <v>0.3</v>
       </c>
@@ -1092,10 +1095,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
         <v>71</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -1153,7 +1159,7 @@
   <sheetPr codeName="Sheet15" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1365,7 +1371,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="155" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1420,7 +1426,7 @@
         <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>21</v>
@@ -1502,7 +1508,7 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
+    <sheetView zoomScale="147" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
       <selection activeCell="I3" sqref="I2:I3"/>
     </sheetView>
   </sheetViews>
@@ -1572,7 +1578,7 @@
         <v>29</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1596,7 +1602,7 @@
         <v>29</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>